<commit_message>
added multithreading to Port Range PY
</commit_message>
<xml_diff>
--- a/Port range VLAN changes.xlsx
+++ b/Port range VLAN changes.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Nextcloud\Root\Python Programs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGit\Github_projects\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF2FA0-3EA7-4516-81D9-2C3CF1BC88B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4035"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Morfe's Network" sheetId="1" r:id="rId1"/>
+    <sheet name="Playbook1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,30 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Floors</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
   <si>
     <t>Metering</t>
   </si>
   <si>
-    <t>switchport 0/20 - 25</t>
-  </si>
-  <si>
-    <t>192.168.10.12</t>
-  </si>
-  <si>
     <t>IP</t>
   </si>
   <si>
     <t>VLAN</t>
+  </si>
+  <si>
+    <t>10.0.252.11</t>
+  </si>
+  <si>
+    <t>Gi1/0/21 - 23</t>
+  </si>
+  <si>
+    <t>CoreIP</t>
+  </si>
+  <si>
+    <t>10.0.252.1</t>
+  </si>
+  <si>
+    <t>CoreTrunk</t>
+  </si>
+  <si>
+    <t>IDFTrunk</t>
+  </si>
+  <si>
+    <t>Floor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,17 +124,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,47 +449,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="3" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>170</v>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed Metering column to Port-Range
</commit_message>
<xml_diff>
--- a/Port range VLAN changes.xlsx
+++ b/Port range VLAN changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGit\Github_projects\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF2FA0-3EA7-4516-81D9-2C3CF1BC88B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C27386-DEA0-4F40-A41E-6C065F4A6473}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19080" yWindow="0" windowWidth="19420" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Playbook1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
-  <si>
-    <t>Metering</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>IP</t>
   </si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>Floor</t>
+  </si>
+  <si>
+    <t>Port-Range</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,40 +468,40 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
       <c r="E2">
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed interface to interface range for Core interface(s) changes and added Description to excel sheet.
</commit_message>
<xml_diff>
--- a/Port range VLAN changes.xlsx
+++ b/Port range VLAN changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyGit\Github_projects\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C27386-DEA0-4F40-A41E-6C065F4A6473}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8733F27-4A40-4367-B0E7-FF52859D204F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19080" yWindow="0" windowWidth="19420" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>IP</t>
   </si>
@@ -51,10 +51,13 @@
     <t>IDFTrunk</t>
   </si>
   <si>
-    <t>Floor</t>
-  </si>
-  <si>
     <t>Port-Range</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>changed from Python Script</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,13 +471,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
@@ -490,7 +493,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>